<commit_message>
Se agrega página de calendario
</commit_message>
<xml_diff>
--- a/Documentacion/Historia de usuario.xlsx
+++ b/Documentacion/Historia de usuario.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rosa Cecilia Nieto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natacha Libreros\Desktop\NATACHA\PROGRAMACION\CICLO 3\SPRINT GRUPO 4\Proyecto-Ciclo-3\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2116E0EA-83C6-40BB-990D-E07D175BFA4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{61FF5218-8723-4EB1-903C-1089B36C135D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -640,7 +639,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m"/>
   </numFmts>
@@ -778,53 +777,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -845,11 +814,41 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1186,14 +1185,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C75681C-E315-4DCA-B074-FCEDBD5320C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J161"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
       <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
@@ -1211,11 +1210,11 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -1233,196 +1232,196 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="2:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="2:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="2:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="10"/>
-      <c r="C11" s="11" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="10"/>
-      <c r="C12" s="11" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
-      <c r="C13" s="11" t="s">
+      <c r="B13" s="22"/>
+      <c r="C13" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="15">
         <v>44256</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="17">
         <v>2</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="17">
         <v>3</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1451,410 +1450,410 @@
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="2:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="2:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="20"/>
+      <c r="E23" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="10"/>
-      <c r="C27" s="11" t="s">
+      <c r="B27" s="22"/>
+      <c r="C27" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="11" t="s">
+      <c r="B28" s="22"/>
+      <c r="C28" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="10"/>
-      <c r="C29" s="11" t="s">
+      <c r="B29" s="22"/>
+      <c r="C29" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="10"/>
-      <c r="C30" s="11" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="15">
         <v>44256</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14" t="s">
+      <c r="D31" s="15"/>
+      <c r="E31" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="17">
         <v>2</v>
       </c>
-      <c r="D32" s="15"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="17">
         <v>3</v>
       </c>
-      <c r="D33" s="15"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="19"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="24"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="22"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="12"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="18" t="s">
+      <c r="A37" s="11"/>
+      <c r="B37" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="22"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="12"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="6" t="s">
+    <row r="38" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="8" t="s">
+      <c r="D38" s="20"/>
+      <c r="E38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="22"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="12"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="9" t="s">
+      <c r="A39" s="11"/>
+      <c r="B39" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="22"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="12"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="9" t="s">
+      <c r="A40" s="11"/>
+      <c r="B40" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="22"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="12"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="10" t="s">
+      <c r="A41" s="11"/>
+      <c r="B41" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="22"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="12"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="10"/>
-      <c r="C42" s="11" t="s">
+      <c r="A42" s="11"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="12"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11" t="s">
+      <c r="A43" s="11"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="22"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="12"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="11" t="s">
+      <c r="A44" s="11"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="22"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="12"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
-      <c r="B45" s="12" t="s">
+      <c r="A45" s="11"/>
+      <c r="B45" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="13">
+      <c r="C45" s="15">
         <v>44256</v>
       </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="14" t="s">
+      <c r="D45" s="15"/>
+      <c r="E45" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="22"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="12"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
-      <c r="B46" s="12" t="s">
+      <c r="A46" s="11"/>
+      <c r="B46" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="17">
         <v>2</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="22"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="12"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="15">
+      <c r="C47" s="17">
         <v>3</v>
       </c>
-      <c r="D47" s="15"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
@@ -1880,188 +1879,188 @@
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="5" t="s">
+      <c r="E52" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="2:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B53" s="6" t="s">
+    <row r="53" spans="2:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="7"/>
-      <c r="E53" s="8" t="s">
+      <c r="D53" s="20"/>
+      <c r="E53" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="9"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="9"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="10"/>
-      <c r="C57" s="11" t="s">
+      <c r="B57" s="22"/>
+      <c r="C57" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="10"/>
-      <c r="C58" s="11" t="s">
+      <c r="B58" s="22"/>
+      <c r="C58" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="10"/>
-      <c r="C59" s="11" t="s">
+      <c r="B59" s="22"/>
+      <c r="C59" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D59" s="11"/>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="13">
+      <c r="C60" s="15">
         <v>44256</v>
       </c>
-      <c r="D60" s="13"/>
-      <c r="E60" s="14" t="s">
+      <c r="D60" s="15"/>
+      <c r="E60" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="15">
+      <c r="C61" s="17">
         <v>2</v>
       </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="15">
+      <c r="C62" s="17">
         <v>3</v>
       </c>
-      <c r="D62" s="15"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -2117,186 +2116,186 @@
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" s="18" t="s">
+      <c r="B70" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="5" t="s">
+      <c r="E70" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
+      <c r="F70" s="25"/>
+      <c r="G70" s="25"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
       <c r="J70" s="1"/>
     </row>
-    <row r="71" spans="2:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B71" s="6" t="s">
+    <row r="71" spans="2:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C71" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D71" s="7"/>
-      <c r="E71" s="8" t="s">
+      <c r="D71" s="20"/>
+      <c r="E71" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
       <c r="J71" s="1"/>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="9"/>
-      <c r="G72" s="9"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
       <c r="J72" s="1"/>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
+      <c r="C73" s="21"/>
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
     </row>
     <row r="74" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="10" t="s">
+      <c r="B74" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
       <c r="J74" s="1"/>
     </row>
     <row r="75" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="10"/>
-      <c r="C75" s="11" t="s">
+      <c r="B75" s="22"/>
+      <c r="C75" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="23"/>
+      <c r="F75" s="23"/>
+      <c r="G75" s="23"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
       <c r="J75" s="1"/>
     </row>
     <row r="76" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="10"/>
-      <c r="C76" s="11" t="s">
+      <c r="B76" s="22"/>
+      <c r="C76" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="10"/>
-      <c r="C77" s="11"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="23"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
     <row r="78" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="13">
+      <c r="C78" s="15">
         <v>44256</v>
       </c>
-      <c r="D78" s="13"/>
-      <c r="E78" s="14" t="s">
+      <c r="D78" s="15"/>
+      <c r="E78" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="F78" s="14"/>
-      <c r="G78" s="14"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
       <c r="J78" s="1"/>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C79" s="15">
+      <c r="C79" s="17">
         <v>2</v>
       </c>
-      <c r="D79" s="15"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="14"/>
-      <c r="G79" s="14"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
       <c r="J79" s="1"/>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C80" s="15">
+      <c r="C80" s="17">
         <v>3</v>
       </c>
-      <c r="D80" s="15"/>
-      <c r="E80" s="14"/>
-      <c r="F80" s="14"/>
-      <c r="G80" s="14"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
@@ -2322,189 +2321,189 @@
       <c r="J82" s="1"/>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
       <c r="J83" s="1"/>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
       <c r="J84" s="1"/>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="18" t="s">
+      <c r="B85" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C85" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="5" t="s">
+      <c r="E85" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="F85" s="5"/>
-      <c r="G85" s="5"/>
+      <c r="F85" s="25"/>
+      <c r="G85" s="25"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
       <c r="J85" s="1"/>
     </row>
-    <row r="86" spans="2:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B86" s="6" t="s">
+    <row r="86" spans="2:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D86" s="7"/>
-      <c r="E86" s="8" t="s">
+      <c r="D86" s="20"/>
+      <c r="E86" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
       <c r="J86" s="1"/>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B87" s="9" t="s">
+      <c r="B87" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9"/>
-      <c r="F87" s="9"/>
-      <c r="G87" s="9"/>
+      <c r="C87" s="21"/>
+      <c r="D87" s="21"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="21"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
       <c r="J87" s="1"/>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="9"/>
+      <c r="C88" s="21"/>
+      <c r="D88" s="21"/>
+      <c r="E88" s="21"/>
+      <c r="F88" s="21"/>
+      <c r="G88" s="21"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
       <c r="J88" s="1"/>
     </row>
     <row r="89" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="10" t="s">
+      <c r="B89" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C89" s="11" t="s">
+      <c r="C89" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
+      <c r="D89" s="23"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="10"/>
-      <c r="C90" s="11" t="s">
+      <c r="B90" s="22"/>
+      <c r="C90" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
+      <c r="D90" s="23"/>
+      <c r="E90" s="23"/>
+      <c r="F90" s="23"/>
+      <c r="G90" s="23"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
       <c r="J90" s="1"/>
     </row>
     <row r="91" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="10"/>
-      <c r="C91" s="11" t="s">
+      <c r="B91" s="22"/>
+      <c r="C91" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B92" s="10"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="11"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="23"/>
+      <c r="D92" s="23"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B93" s="12" t="s">
+      <c r="B93" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C93" s="13">
+      <c r="C93" s="15">
         <v>44256</v>
       </c>
-      <c r="D93" s="13"/>
-      <c r="E93" s="14" t="s">
+      <c r="D93" s="15"/>
+      <c r="E93" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F93" s="14"/>
-      <c r="G93" s="14"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="16"/>
       <c r="H93" s="1"/>
-      <c r="I93" s="24"/>
+      <c r="I93" s="14"/>
       <c r="J93" s="1"/>
     </row>
     <row r="94" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="12" t="s">
+      <c r="B94" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C94" s="15">
+      <c r="C94" s="17">
         <v>2</v>
       </c>
-      <c r="D94" s="15"/>
-      <c r="E94" s="14"/>
-      <c r="F94" s="14"/>
-      <c r="G94" s="14"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="16"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="16"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
       <c r="J94" s="1"/>
     </row>
     <row r="95" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="12" t="s">
+      <c r="B95" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C95" s="15">
+      <c r="C95" s="17">
         <v>3</v>
       </c>
-      <c r="D95" s="15"/>
-      <c r="E95" s="14"/>
-      <c r="F95" s="14"/>
-      <c r="G95" s="14"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="16"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="16"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
-      <c r="J95" s="23"/>
+      <c r="J95" s="13"/>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C96" s="1"/>
@@ -2547,186 +2546,186 @@
       <c r="J99" s="1"/>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
       <c r="J100" s="1"/>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
+      <c r="B101" s="24"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
     </row>
     <row r="102" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="18" t="s">
+      <c r="B102" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D102" s="3" t="s">
+      <c r="D102" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E102" s="5" t="s">
+      <c r="E102" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F102" s="5"/>
-      <c r="G102" s="5"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="25"/>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
       <c r="J102" s="1"/>
     </row>
     <row r="103" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="6" t="s">
+      <c r="B103" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C103" s="7" t="s">
+      <c r="C103" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D103" s="7"/>
-      <c r="E103" s="8" t="s">
+      <c r="D103" s="20"/>
+      <c r="E103" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F103" s="7"/>
-      <c r="G103" s="7"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="20"/>
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B104" s="9" t="s">
+      <c r="B104" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="9"/>
-      <c r="G104" s="9"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="21"/>
+      <c r="E104" s="21"/>
+      <c r="F104" s="21"/>
+      <c r="G104" s="21"/>
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
       <c r="J104" s="1"/>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B105" s="9" t="s">
+      <c r="B105" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C105" s="9"/>
-      <c r="D105" s="9"/>
-      <c r="E105" s="9"/>
-      <c r="F105" s="9"/>
-      <c r="G105" s="9"/>
+      <c r="C105" s="21"/>
+      <c r="D105" s="21"/>
+      <c r="E105" s="21"/>
+      <c r="F105" s="21"/>
+      <c r="G105" s="21"/>
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
       <c r="J105" s="1"/>
     </row>
     <row r="106" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="10" t="s">
+      <c r="B106" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C106" s="11" t="s">
+      <c r="C106" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
+      <c r="D106" s="23"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="23"/>
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
       <c r="J106" s="1"/>
     </row>
     <row r="107" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="10"/>
-      <c r="C107" s="11" t="s">
+      <c r="B107" s="22"/>
+      <c r="C107" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
+      <c r="D107" s="23"/>
+      <c r="E107" s="23"/>
+      <c r="F107" s="23"/>
+      <c r="G107" s="23"/>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
     </row>
     <row r="108" spans="2:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="10"/>
-      <c r="C108" s="11" t="s">
+      <c r="B108" s="22"/>
+      <c r="C108" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="D108" s="11"/>
-      <c r="E108" s="11"/>
-      <c r="F108" s="11"/>
-      <c r="G108" s="11"/>
+      <c r="D108" s="23"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="23"/>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
       <c r="J108" s="1"/>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B109" s="10"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
-      <c r="G109" s="11"/>
+      <c r="B109" s="22"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="23"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="23"/>
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
       <c r="J109" s="1"/>
     </row>
     <row r="110" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="12" t="s">
+      <c r="B110" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C110" s="13">
+      <c r="C110" s="15">
         <v>44256</v>
       </c>
-      <c r="D110" s="13"/>
-      <c r="E110" s="14" t="s">
+      <c r="D110" s="15"/>
+      <c r="E110" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="F110" s="14"/>
-      <c r="G110" s="14"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
       <c r="J110" s="1"/>
     </row>
     <row r="111" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="12" t="s">
+      <c r="B111" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C111" s="15">
+      <c r="C111" s="17">
         <v>2</v>
       </c>
-      <c r="D111" s="15"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="14"/>
-      <c r="G111" s="14"/>
+      <c r="D111" s="17"/>
+      <c r="E111" s="16"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="16"/>
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
       <c r="J111" s="1"/>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B112" s="12" t="s">
+      <c r="B112" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C112" s="15">
+      <c r="C112" s="17">
         <v>3</v>
       </c>
-      <c r="D112" s="15"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
-      <c r="G112" s="14"/>
+      <c r="D112" s="17"/>
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
       <c r="H112" s="1"/>
       <c r="I112" s="1"/>
       <c r="J112" s="1"/>
@@ -2762,184 +2761,184 @@
       <c r="J115" s="1"/>
     </row>
     <row r="116" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="24"/>
+      <c r="F116" s="24"/>
+      <c r="G116" s="24"/>
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
       <c r="J116" s="1"/>
     </row>
     <row r="117" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2"/>
+      <c r="B117" s="24"/>
+      <c r="C117" s="24"/>
+      <c r="D117" s="24"/>
+      <c r="E117" s="24"/>
+      <c r="F117" s="24"/>
+      <c r="G117" s="24"/>
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
       <c r="J117" s="1"/>
     </row>
     <row r="118" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B118" s="18" t="s">
+      <c r="B118" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C118" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D118" s="3" t="s">
+      <c r="D118" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E118" s="5" t="s">
+      <c r="E118" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
+      <c r="F118" s="25"/>
+      <c r="G118" s="25"/>
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
       <c r="J118" s="1"/>
     </row>
-    <row r="119" spans="2:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B119" s="6" t="s">
+    <row r="119" spans="2:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C119" s="7" t="s">
+      <c r="C119" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D119" s="7"/>
-      <c r="E119" s="8" t="s">
+      <c r="D119" s="20"/>
+      <c r="E119" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F119" s="7"/>
-      <c r="G119" s="7"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="20"/>
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
       <c r="J119" s="1"/>
     </row>
     <row r="120" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B120" s="9" t="s">
+      <c r="B120" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
+      <c r="C120" s="21"/>
+      <c r="D120" s="21"/>
+      <c r="E120" s="21"/>
+      <c r="F120" s="21"/>
+      <c r="G120" s="21"/>
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
       <c r="J120" s="1"/>
     </row>
     <row r="121" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B121" s="9" t="s">
+      <c r="B121" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C121" s="9"/>
-      <c r="D121" s="9"/>
-      <c r="E121" s="9"/>
-      <c r="F121" s="9"/>
-      <c r="G121" s="9"/>
+      <c r="C121" s="21"/>
+      <c r="D121" s="21"/>
+      <c r="E121" s="21"/>
+      <c r="F121" s="21"/>
+      <c r="G121" s="21"/>
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
       <c r="J121" s="1"/>
     </row>
     <row r="122" spans="2:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="10" t="s">
+      <c r="B122" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C122" s="11" t="s">
+      <c r="C122" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="D122" s="11"/>
-      <c r="E122" s="11"/>
-      <c r="F122" s="11"/>
-      <c r="G122" s="11"/>
+      <c r="D122" s="23"/>
+      <c r="E122" s="23"/>
+      <c r="F122" s="23"/>
+      <c r="G122" s="23"/>
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
       <c r="J122" s="1"/>
     </row>
     <row r="123" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B123" s="10"/>
-      <c r="C123" s="11" t="s">
+      <c r="B123" s="22"/>
+      <c r="C123" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D123" s="11"/>
-      <c r="E123" s="11"/>
-      <c r="F123" s="11"/>
-      <c r="G123" s="11"/>
+      <c r="D123" s="23"/>
+      <c r="E123" s="23"/>
+      <c r="F123" s="23"/>
+      <c r="G123" s="23"/>
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
       <c r="J123" s="1"/>
     </row>
     <row r="124" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B124" s="10"/>
-      <c r="C124" s="11"/>
-      <c r="D124" s="11"/>
-      <c r="E124" s="11"/>
-      <c r="F124" s="11"/>
-      <c r="G124" s="11"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="23"/>
+      <c r="D124" s="23"/>
+      <c r="E124" s="23"/>
+      <c r="F124" s="23"/>
+      <c r="G124" s="23"/>
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
       <c r="J124" s="1"/>
     </row>
     <row r="125" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B125" s="10"/>
-      <c r="C125" s="11"/>
-      <c r="D125" s="11"/>
-      <c r="E125" s="11"/>
-      <c r="F125" s="11"/>
-      <c r="G125" s="11"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="23"/>
+      <c r="D125" s="23"/>
+      <c r="E125" s="23"/>
+      <c r="F125" s="23"/>
+      <c r="G125" s="23"/>
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
       <c r="J125" s="1"/>
     </row>
     <row r="126" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="12" t="s">
+      <c r="B126" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C126" s="13">
+      <c r="C126" s="15">
         <v>44256</v>
       </c>
-      <c r="D126" s="13"/>
-      <c r="E126" s="14" t="s">
+      <c r="D126" s="15"/>
+      <c r="E126" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
     </row>
     <row r="127" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B127" s="12" t="s">
+      <c r="B127" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C127" s="15">
+      <c r="C127" s="17">
         <v>2</v>
       </c>
-      <c r="D127" s="15"/>
-      <c r="E127" s="14"/>
-      <c r="F127" s="14"/>
-      <c r="G127" s="14"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="16"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="16"/>
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
       <c r="J127" s="1"/>
     </row>
     <row r="128" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B128" s="12" t="s">
+      <c r="B128" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C128" s="15">
+      <c r="C128" s="17">
         <v>3</v>
       </c>
-      <c r="D128" s="15"/>
-      <c r="E128" s="14"/>
-      <c r="F128" s="14"/>
-      <c r="G128" s="14"/>
+      <c r="D128" s="17"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="16"/>
+      <c r="G128" s="16"/>
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
       <c r="J128" s="1"/>
@@ -2975,186 +2974,186 @@
       <c r="J131" s="1"/>
     </row>
     <row r="132" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B132" s="2" t="s">
+      <c r="B132" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C132" s="2"/>
-      <c r="D132" s="2"/>
-      <c r="E132" s="2"/>
-      <c r="F132" s="2"/>
-      <c r="G132" s="2"/>
+      <c r="C132" s="24"/>
+      <c r="D132" s="24"/>
+      <c r="E132" s="24"/>
+      <c r="F132" s="24"/>
+      <c r="G132" s="24"/>
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
       <c r="J132" s="1"/>
     </row>
     <row r="133" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="2"/>
-      <c r="E133" s="2"/>
-      <c r="F133" s="2"/>
-      <c r="G133" s="2"/>
+      <c r="B133" s="24"/>
+      <c r="C133" s="24"/>
+      <c r="D133" s="24"/>
+      <c r="E133" s="24"/>
+      <c r="F133" s="24"/>
+      <c r="G133" s="24"/>
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
       <c r="J133" s="1"/>
     </row>
     <row r="134" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B134" s="18" t="s">
+      <c r="B134" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C134" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D134" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E134" s="5" t="s">
+      <c r="E134" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F134" s="5"/>
-      <c r="G134" s="5"/>
+      <c r="F134" s="25"/>
+      <c r="G134" s="25"/>
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
       <c r="J134" s="1"/>
     </row>
-    <row r="135" spans="2:10" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B135" s="6" t="s">
+    <row r="135" spans="2:10" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C135" s="7" t="s">
+      <c r="C135" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D135" s="7"/>
-      <c r="E135" s="8" t="s">
+      <c r="D135" s="20"/>
+      <c r="E135" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F135" s="7"/>
-      <c r="G135" s="7"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="20"/>
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
       <c r="J135" s="1"/>
     </row>
     <row r="136" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B136" s="9" t="s">
+      <c r="B136" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C136" s="9"/>
-      <c r="D136" s="9"/>
-      <c r="E136" s="9"/>
-      <c r="F136" s="9"/>
-      <c r="G136" s="9"/>
+      <c r="C136" s="21"/>
+      <c r="D136" s="21"/>
+      <c r="E136" s="21"/>
+      <c r="F136" s="21"/>
+      <c r="G136" s="21"/>
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
       <c r="J136" s="1"/>
     </row>
     <row r="137" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B137" s="9" t="s">
+      <c r="B137" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C137" s="9"/>
-      <c r="D137" s="9"/>
-      <c r="E137" s="9"/>
-      <c r="F137" s="9"/>
-      <c r="G137" s="9"/>
+      <c r="C137" s="21"/>
+      <c r="D137" s="21"/>
+      <c r="E137" s="21"/>
+      <c r="F137" s="21"/>
+      <c r="G137" s="21"/>
       <c r="H137" s="1"/>
       <c r="I137" s="1"/>
       <c r="J137" s="1"/>
     </row>
     <row r="138" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B138" s="10" t="s">
+      <c r="B138" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C138" s="11" t="s">
+      <c r="C138" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D138" s="11"/>
-      <c r="E138" s="11"/>
-      <c r="F138" s="11"/>
-      <c r="G138" s="11"/>
+      <c r="D138" s="23"/>
+      <c r="E138" s="23"/>
+      <c r="F138" s="23"/>
+      <c r="G138" s="23"/>
       <c r="H138" s="1"/>
       <c r="I138" s="1"/>
       <c r="J138" s="1"/>
     </row>
     <row r="139" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B139" s="10"/>
-      <c r="C139" s="11" t="s">
+      <c r="B139" s="22"/>
+      <c r="C139" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="D139" s="11"/>
-      <c r="E139" s="11"/>
-      <c r="F139" s="11"/>
-      <c r="G139" s="11"/>
+      <c r="D139" s="23"/>
+      <c r="E139" s="23"/>
+      <c r="F139" s="23"/>
+      <c r="G139" s="23"/>
       <c r="H139" s="1"/>
       <c r="I139" s="1"/>
       <c r="J139" s="1"/>
     </row>
     <row r="140" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B140" s="10"/>
-      <c r="C140" s="11" t="s">
+      <c r="B140" s="22"/>
+      <c r="C140" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D140" s="11"/>
-      <c r="E140" s="11"/>
-      <c r="F140" s="11"/>
-      <c r="G140" s="11"/>
+      <c r="D140" s="23"/>
+      <c r="E140" s="23"/>
+      <c r="F140" s="23"/>
+      <c r="G140" s="23"/>
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
       <c r="J140" s="1"/>
     </row>
     <row r="141" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B141" s="10"/>
-      <c r="C141" s="11"/>
-      <c r="D141" s="11"/>
-      <c r="E141" s="11"/>
-      <c r="F141" s="11"/>
-      <c r="G141" s="11"/>
+      <c r="B141" s="22"/>
+      <c r="C141" s="23"/>
+      <c r="D141" s="23"/>
+      <c r="E141" s="23"/>
+      <c r="F141" s="23"/>
+      <c r="G141" s="23"/>
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
       <c r="J141" s="1"/>
     </row>
     <row r="142" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="12" t="s">
+      <c r="B142" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C142" s="13">
+      <c r="C142" s="15">
         <v>44256</v>
       </c>
-      <c r="D142" s="13"/>
-      <c r="E142" s="14" t="s">
+      <c r="D142" s="15"/>
+      <c r="E142" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="F142" s="14"/>
-      <c r="G142" s="14"/>
+      <c r="F142" s="16"/>
+      <c r="G142" s="16"/>
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
       <c r="J142" s="1"/>
     </row>
     <row r="143" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="12" t="s">
+      <c r="B143" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C143" s="15">
+      <c r="C143" s="17">
         <v>2</v>
       </c>
-      <c r="D143" s="15"/>
-      <c r="E143" s="14"/>
-      <c r="F143" s="14"/>
-      <c r="G143" s="14"/>
+      <c r="D143" s="17"/>
+      <c r="E143" s="16"/>
+      <c r="F143" s="16"/>
+      <c r="G143" s="16"/>
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
       <c r="J143" s="1"/>
     </row>
     <row r="144" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B144" s="12" t="s">
+      <c r="B144" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C144" s="15">
+      <c r="C144" s="17">
         <v>3</v>
       </c>
-      <c r="D144" s="15"/>
-      <c r="E144" s="14"/>
-      <c r="F144" s="14"/>
-      <c r="G144" s="14"/>
+      <c r="D144" s="17"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
       <c r="J144" s="1"/>
@@ -3211,6 +3210,120 @@
     </row>
   </sheetData>
   <mergeCells count="138">
+    <mergeCell ref="B4:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B20:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="B24:G24"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="E14:G16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="B35:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:G47"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="B50:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="E60:G62"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="B68:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:G80"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="B83:G84"/>
+    <mergeCell ref="E85:G85"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="B74:B77"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="C75:G75"/>
+    <mergeCell ref="C76:G76"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="E93:G95"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="B100:G101"/>
+    <mergeCell ref="E102:G102"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="B87:G87"/>
+    <mergeCell ref="B88:G88"/>
+    <mergeCell ref="B89:B92"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="C91:G91"/>
+    <mergeCell ref="C92:G92"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="F103:G103"/>
+    <mergeCell ref="B104:G104"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B106:B109"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="C107:G107"/>
+    <mergeCell ref="C108:G108"/>
+    <mergeCell ref="C109:G109"/>
+    <mergeCell ref="B122:B125"/>
+    <mergeCell ref="C122:G122"/>
+    <mergeCell ref="C123:G123"/>
+    <mergeCell ref="C124:G124"/>
+    <mergeCell ref="C125:G125"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="E110:G112"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="B116:G117"/>
+    <mergeCell ref="E118:G118"/>
     <mergeCell ref="C142:D142"/>
     <mergeCell ref="E142:G144"/>
     <mergeCell ref="C143:D143"/>
@@ -3235,120 +3348,6 @@
     <mergeCell ref="F119:G119"/>
     <mergeCell ref="B120:G120"/>
     <mergeCell ref="B121:G121"/>
-    <mergeCell ref="B122:B125"/>
-    <mergeCell ref="C122:G122"/>
-    <mergeCell ref="C123:G123"/>
-    <mergeCell ref="C124:G124"/>
-    <mergeCell ref="C125:G125"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="E110:G112"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="B116:G117"/>
-    <mergeCell ref="E118:G118"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="F103:G103"/>
-    <mergeCell ref="B104:G104"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B106:B109"/>
-    <mergeCell ref="C106:G106"/>
-    <mergeCell ref="C107:G107"/>
-    <mergeCell ref="C108:G108"/>
-    <mergeCell ref="C109:G109"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="E93:G95"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="B100:G101"/>
-    <mergeCell ref="E102:G102"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="B87:G87"/>
-    <mergeCell ref="B88:G88"/>
-    <mergeCell ref="B89:B92"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="C91:G91"/>
-    <mergeCell ref="C92:G92"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:G80"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="B83:G84"/>
-    <mergeCell ref="E85:G85"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="B74:B77"/>
-    <mergeCell ref="C74:G74"/>
-    <mergeCell ref="C75:G75"/>
-    <mergeCell ref="C76:G76"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="E60:G62"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="B68:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:G47"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="B50:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="C44:G44"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="B35:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="C27:G27"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B20:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="E14:G16"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B4:G5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
   </mergeCells>
   <conditionalFormatting sqref="E6 E70 E85 E102 E118 E134 E52:E53 E22">
     <cfRule type="expression" dxfId="2" priority="1">

</xml_diff>